<commit_message>
Fin pratique labo 2 + clean
</commit_message>
<xml_diff>
--- a/Excercices/01_Speech_HMM/Tab.xlsx
+++ b/Excercices/01_Speech_HMM/Tab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\S1\MPRI\Excercices\01_Speech_HMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FF289F-2937-4A49-9E4F-3E07FCF50347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C32E7E3-4EA1-4C12-81F6-EE86CEB59290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
   <si>
     <t>Mot</t>
   </si>
@@ -55,15 +55,122 @@
   </si>
   <si>
     <t>cinq</t>
+  </si>
+  <si>
+    <t>ɛ̃</t>
+  </si>
+  <si>
+    <t>dø</t>
+  </si>
+  <si>
+    <t>tʁwa</t>
+  </si>
+  <si>
+    <t>katʁ</t>
+  </si>
+  <si>
+    <t>sɛ̃k</t>
+  </si>
+  <si>
+    <t>2 240</t>
+  </si>
+  <si>
+    <t>1 965</t>
+  </si>
+  <si>
+    <t>2 025</t>
+  </si>
+  <si>
+    <t>2 265</t>
+  </si>
+  <si>
+    <t>2 225</t>
+  </si>
+  <si>
+    <t>Mot testé</t>
+  </si>
+  <si>
+    <t>peu</t>
+  </si>
+  <si>
+    <t>Valeurs des probabilités</t>
+  </si>
+  <si>
+    <t>Modèle 1</t>
+  </si>
+  <si>
+    <t>Modèle 2</t>
+  </si>
+  <si>
+    <t>Modèle 3</t>
+  </si>
+  <si>
+    <t>Modèle 4</t>
+  </si>
+  <si>
+    <t>Modèle 5</t>
+  </si>
+  <si>
+    <t>Modèle simple</t>
+  </si>
+  <si>
+    <t>Modèle LTR</t>
+  </si>
+  <si>
+    <t>(fichier collègue)</t>
+  </si>
+  <si>
+    <t>(pas stable)</t>
+  </si>
+  <si>
+    <t>(stable)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -138,11 +245,304 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -155,6 +555,156 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I41" sqref="I41:N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,9 +998,10 @@
     <col min="3" max="3" width="4.88671875" customWidth="1"/>
     <col min="4" max="4" width="9.21875" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,53 +1017,835 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <v>280</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4">
+        <v>246</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4">
+        <v>253</v>
+      </c>
+      <c r="I4" s="38"/>
+      <c r="J4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
+        <v>283</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4">
+        <v>278</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="40">
+        <v>1</v>
+      </c>
+      <c r="J6" s="35">
+        <v>-2475.1393225061101</v>
+      </c>
+      <c r="K6" s="24">
+        <v>-5148.1722299399999</v>
+      </c>
+      <c r="L6" s="22">
+        <v>-4149.5922209999999</v>
+      </c>
+      <c r="M6" s="22">
+        <v>-5101.3932199999999</v>
+      </c>
+      <c r="N6" s="25">
+        <v>-6537.384</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H7" s="5"/>
+      <c r="I7" s="40">
+        <v>2</v>
+      </c>
+      <c r="J7" s="36">
+        <v>-3822.5064662499999</v>
+      </c>
+      <c r="K7" s="23">
+        <v>-1590.9455519000001</v>
+      </c>
+      <c r="L7" s="22">
+        <v>-4626.2904769999996</v>
+      </c>
+      <c r="M7" s="22">
+        <v>-4255.366</v>
+      </c>
+      <c r="N7" s="25">
+        <v>-5781.09</v>
+      </c>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H8" s="5"/>
+      <c r="I8" s="40">
+        <v>3</v>
+      </c>
+      <c r="J8" s="36">
+        <v>-3421.9438500000001</v>
+      </c>
+      <c r="K8" s="22">
+        <v>-5662.759</v>
+      </c>
+      <c r="L8" s="23">
+        <v>-2115.7037599999999</v>
+      </c>
+      <c r="M8" s="22">
+        <v>-5352.2494999999999</v>
+      </c>
+      <c r="N8" s="25">
+        <v>-6679.6710739999999</v>
+      </c>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H9" s="5"/>
+      <c r="I9" s="40">
+        <v>4</v>
+      </c>
+      <c r="J9" s="36">
+        <v>-4856.2</v>
+      </c>
+      <c r="K9" s="22">
+        <v>-5189.6850000000004</v>
+      </c>
+      <c r="L9" s="22">
+        <v>-5393.2155000000002</v>
+      </c>
+      <c r="M9" s="23">
+        <v>-2896.5983000000001</v>
+      </c>
+      <c r="N9" s="25">
+        <v>-5301.9645257000002</v>
+      </c>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H10" s="5"/>
+      <c r="I10" s="40">
+        <v>5</v>
+      </c>
+      <c r="J10" s="36">
+        <v>-4454.7650000000003</v>
+      </c>
+      <c r="K10" s="22">
+        <v>-5794.0302226000003</v>
+      </c>
+      <c r="L10" s="22">
+        <v>-5571.79</v>
+      </c>
+      <c r="M10" s="22">
+        <v>-6273.3140000000003</v>
+      </c>
+      <c r="N10" s="26">
+        <v>-2515.0571073000001</v>
+      </c>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="5"/>
+      <c r="I11" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="37">
+        <v>-4372.1048000000001</v>
+      </c>
+      <c r="K11" s="28">
+        <v>-3345.0918999999999</v>
+      </c>
+      <c r="L11" s="27">
+        <v>-5745.8347999999996</v>
+      </c>
+      <c r="M11" s="27">
+        <v>-4949.0599782700001</v>
+      </c>
+      <c r="N11" s="29">
+        <v>-4557.8014000000003</v>
+      </c>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H13" s="5"/>
+      <c r="I13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H14" s="5"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="12"/>
+      <c r="J16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I18" s="39">
+        <v>1</v>
+      </c>
+      <c r="J18" s="43">
+        <v>-3227.0763999999999</v>
+      </c>
+      <c r="K18" s="30">
+        <v>-5025.9665000000005</v>
+      </c>
+      <c r="L18" s="30">
+        <v>-4026.9553000000001</v>
+      </c>
+      <c r="M18" s="30">
+        <v>-4879.5256006999998</v>
+      </c>
+      <c r="N18" s="31">
+        <v>-5909.7089999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I19" s="40">
+        <v>2</v>
+      </c>
+      <c r="J19" s="36">
+        <v>-4081.2507999999998</v>
+      </c>
+      <c r="K19" s="23">
+        <v>-2348.3851</v>
+      </c>
+      <c r="L19" s="22">
+        <v>-4026.003604</v>
+      </c>
+      <c r="M19" s="22">
+        <v>-4346.1591330000001</v>
+      </c>
+      <c r="N19" s="25">
+        <v>-4495.9229743879496</v>
+      </c>
+    </row>
+    <row r="20" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I20" s="40">
+        <v>3</v>
+      </c>
+      <c r="J20" s="36">
+        <v>-4653.1549999999997</v>
+      </c>
+      <c r="K20" s="22">
+        <v>-5260.1459000000004</v>
+      </c>
+      <c r="L20" s="23">
+        <v>-3388.9328799999998</v>
+      </c>
+      <c r="M20" s="22">
+        <v>-4945.1123610000004</v>
+      </c>
+      <c r="N20" s="25">
+        <v>-5302.3310000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I21" s="40">
+        <v>4</v>
+      </c>
+      <c r="J21" s="36">
+        <v>-6434.2556999999997</v>
+      </c>
+      <c r="K21" s="22">
+        <v>-5738.2177000000001</v>
+      </c>
+      <c r="L21" s="22">
+        <v>-5430.556799</v>
+      </c>
+      <c r="M21" s="23">
+        <v>-3548.236085</v>
+      </c>
+      <c r="N21" s="25">
+        <v>-5499.6416300000001</v>
+      </c>
+    </row>
+    <row r="22" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I22" s="40">
+        <v>5</v>
+      </c>
+      <c r="J22" s="36">
+        <v>-5438.5482000000002</v>
+      </c>
+      <c r="K22" s="22">
+        <v>-5551.2226000000001</v>
+      </c>
+      <c r="L22" s="22">
+        <v>-4862.9616999999998</v>
+      </c>
+      <c r="M22" s="22">
+        <v>-4798.8664799999997</v>
+      </c>
+      <c r="N22" s="26">
+        <v>-2918.23621</v>
+      </c>
+    </row>
+    <row r="23" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="37">
+        <v>-5006.0484200000001</v>
+      </c>
+      <c r="K23" s="28">
+        <v>-3737.9674599999998</v>
+      </c>
+      <c r="L23" s="27">
+        <v>-5926.1274100000001</v>
+      </c>
+      <c r="M23" s="27">
+        <v>-4205.2629299999999</v>
+      </c>
+      <c r="N23" s="29">
+        <v>-5962.9531939999997</v>
+      </c>
+    </row>
+    <row r="24" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I27" s="12"/>
+      <c r="J27" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="12"/>
+      <c r="J28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N29" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I30" s="39">
+        <v>1</v>
+      </c>
+      <c r="J30" s="43">
+        <v>-4745.18</v>
+      </c>
+      <c r="K30" s="30">
+        <v>-6375.65</v>
+      </c>
+      <c r="L30" s="30">
+        <v>-7292.6212999999998</v>
+      </c>
+      <c r="M30" s="30">
+        <v>-5563.04</v>
+      </c>
+      <c r="N30" s="31">
+        <v>-7841.7443999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I31" s="40">
+        <v>2</v>
+      </c>
+      <c r="J31" s="36">
+        <v>-7046.2448000000004</v>
+      </c>
+      <c r="K31" s="23">
+        <v>-6207.22</v>
+      </c>
+      <c r="L31" s="22">
+        <v>-8773.01</v>
+      </c>
+      <c r="M31" s="22">
+        <v>-7749.0770000000002</v>
+      </c>
+      <c r="N31" s="25">
+        <v>-11626.91742</v>
+      </c>
+    </row>
+    <row r="32" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I32" s="40">
+        <v>3</v>
+      </c>
+      <c r="J32" s="49">
+        <v>-2453.94</v>
+      </c>
+      <c r="K32" s="22">
+        <v>-3891.5186100000001</v>
+      </c>
+      <c r="L32" s="46">
+        <v>-3295.2669999999998</v>
+      </c>
+      <c r="M32" s="22">
+        <v>-4081.04952</v>
+      </c>
+      <c r="N32" s="25">
+        <v>-4954.2960000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I33" s="40">
+        <v>4</v>
+      </c>
+      <c r="J33" s="36">
+        <v>-4022.9490000000001</v>
+      </c>
+      <c r="K33" s="22">
+        <v>-4778.744232</v>
+      </c>
+      <c r="L33" s="22">
+        <v>-5138.6769999999997</v>
+      </c>
+      <c r="M33" s="23">
+        <v>-3626.4729050000001</v>
+      </c>
+      <c r="N33" s="25">
+        <v>-6349.5770000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="41">
+        <v>5</v>
+      </c>
+      <c r="J34" s="50">
+        <v>-4356.9440000000004</v>
+      </c>
+      <c r="K34" s="27">
+        <v>-4433.13771</v>
+      </c>
+      <c r="L34" s="27">
+        <v>-5998.0747629999996</v>
+      </c>
+      <c r="M34" s="27">
+        <v>-4849.57</v>
+      </c>
+      <c r="N34" s="48">
+        <v>-5664.9369999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I35" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="16"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="18"/>
+    </row>
+    <row r="36" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="11"/>
+    </row>
+    <row r="39" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I39" s="12"/>
+      <c r="J39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="14"/>
+    </row>
+    <row r="40" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="12"/>
+      <c r="J40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N40" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I41" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N41" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I42" s="39">
+        <v>1</v>
+      </c>
+      <c r="J42" s="52">
+        <v>-5943.5630000000001</v>
+      </c>
+      <c r="K42" s="51">
+        <v>-5435.4480999999996</v>
+      </c>
+      <c r="L42" s="51">
+        <v>-5315.6760000000004</v>
+      </c>
+      <c r="M42" s="51">
+        <v>-6541.4861000000001</v>
+      </c>
+      <c r="N42" s="54">
+        <v>-4330.4567999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I43" s="40">
+        <v>2</v>
+      </c>
+      <c r="J43" s="53">
+        <v>-9832.2783999999992</v>
+      </c>
+      <c r="K43" s="23">
+        <v>-5895.3040000000001</v>
+      </c>
+      <c r="L43" s="46">
+        <v>-9323.5962</v>
+      </c>
+      <c r="M43" s="46">
+        <v>-8515.0631699999994</v>
+      </c>
+      <c r="N43" s="55">
+        <v>-6197.1240399999997</v>
+      </c>
+    </row>
+    <row r="44" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I44" s="40">
+        <v>3</v>
+      </c>
+      <c r="J44" s="53">
+        <v>-3243.2080000000001</v>
+      </c>
+      <c r="K44" s="46">
+        <v>-3552.9650000000001</v>
+      </c>
+      <c r="L44" s="46">
+        <v>-3577.0654</v>
+      </c>
+      <c r="M44" s="46">
+        <v>-4721.6719999999996</v>
+      </c>
+      <c r="N44" s="56">
+        <v>-3157.0030000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I45" s="40">
+        <v>4</v>
+      </c>
+      <c r="J45" s="53">
+        <v>-5082.0676999999996</v>
+      </c>
+      <c r="K45" s="45">
+        <v>-4121.6420600000001</v>
+      </c>
+      <c r="L45" s="46">
+        <v>-5604.7421100000001</v>
+      </c>
+      <c r="M45" s="46">
+        <v>-4497.2911800000002</v>
+      </c>
+      <c r="N45" s="55">
+        <v>-4368.1241600000003</v>
+      </c>
+    </row>
+    <row r="46" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I46" s="41">
+        <v>5</v>
+      </c>
+      <c r="J46" s="57">
+        <v>-5853.49</v>
+      </c>
+      <c r="K46" s="47">
+        <v>-4180.3262000000004</v>
+      </c>
+      <c r="L46" s="58">
+        <v>-6009.5437300000003</v>
+      </c>
+      <c r="M46" s="58">
+        <v>-6030.0429999999997</v>
+      </c>
+      <c r="N46" s="48">
+        <v>-4240.8100000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I47" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J47" s="16"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I3:N3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>